<commit_message>
Update UML with all module tables
</commit_message>
<xml_diff>
--- a/SupportingDocuments/UML.xlsx
+++ b/SupportingDocuments/UML.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="152">
   <si>
     <t>Job</t>
   </si>
@@ -117,12 +117,6 @@
     <t>map: ProvinceMap</t>
   </si>
   <si>
-    <t>toJob: void</t>
-  </si>
-  <si>
-    <t>getJobArray(): ArrayList&lt;Job&gt;</t>
-  </si>
-  <si>
     <t>Province</t>
   </si>
   <si>
@@ -199,6 +193,285 @@
   </si>
   <si>
     <t>getBackward(String key)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>cityName: String</t>
+  </si>
+  <si>
+    <t>province: Province</t>
+  </si>
+  <si>
+    <t>cityOutlook: Outlook</t>
+  </si>
+  <si>
+    <t>income: double</t>
+  </si>
+  <si>
+    <t>getCityName()</t>
+  </si>
+  <si>
+    <t>getProvince()</t>
+  </si>
+  <si>
+    <t>toJob</t>
+  </si>
+  <si>
+    <t>getJobArray()</t>
+  </si>
+  <si>
+    <t>getOutlook()</t>
+  </si>
+  <si>
+    <t>setOutlook()</t>
+  </si>
+  <si>
+    <t>searchCity(ArrayList&lt;City&gt; cities)</t>
+  </si>
+  <si>
+    <t>compareTo(Object that)</t>
+  </si>
+  <si>
+    <t>getIncome()</t>
+  </si>
+  <si>
+    <t>CityData</t>
+  </si>
+  <si>
+    <t>year: int</t>
+  </si>
+  <si>
+    <t>city: String</t>
+  </si>
+  <si>
+    <t>province: String</t>
+  </si>
+  <si>
+    <t>GeographicalID: String</t>
+  </si>
+  <si>
+    <t>DataType: String</t>
+  </si>
+  <si>
+    <t>Vector: String</t>
+  </si>
+  <si>
+    <t>Coordinate: double</t>
+  </si>
+  <si>
+    <t>Income: double</t>
+  </si>
+  <si>
+    <t>getCoordinate()</t>
+  </si>
+  <si>
+    <t>getDataType()</t>
+  </si>
+  <si>
+    <t>getGeographicalID()</t>
+  </si>
+  <si>
+    <t>getCity()</t>
+  </si>
+  <si>
+    <t>getVector()</t>
+  </si>
+  <si>
+    <t>getYear()</t>
+  </si>
+  <si>
+    <t>CityGraph</t>
+  </si>
+  <si>
+    <t>SCALING_FACTOR: double</t>
+  </si>
+  <si>
+    <t>CITIES_TO_RETURN: int</t>
+  </si>
+  <si>
+    <t>crawlDummies(GraphVertex source, double targetValue)</t>
+  </si>
+  <si>
+    <t>getRelatedCities(City toFind)</t>
+  </si>
+  <si>
+    <t>CityIncome</t>
+  </si>
+  <si>
+    <t>incomes: ArrayList&lt;Double&gt;</t>
+  </si>
+  <si>
+    <t>avgIncome: double</t>
+  </si>
+  <si>
+    <t>getIncomes()</t>
+  </si>
+  <si>
+    <t>addIncome(double income)</t>
+  </si>
+  <si>
+    <t>getAvgIncome()</t>
+  </si>
+  <si>
+    <t>GraphEdge</t>
+  </si>
+  <si>
+    <t>v: GraphVertex</t>
+  </si>
+  <si>
+    <t>w: GraphVertex</t>
+  </si>
+  <si>
+    <t>weight: long</t>
+  </si>
+  <si>
+    <t>getConnection(GraphVertex c)</t>
+  </si>
+  <si>
+    <t>getWeight()</t>
+  </si>
+  <si>
+    <t>compareTo(Object oThat)</t>
+  </si>
+  <si>
+    <t>GraphVertex</t>
+  </si>
+  <si>
+    <t>city: City</t>
+  </si>
+  <si>
+    <t>outlook: double</t>
+  </si>
+  <si>
+    <t>adj: ArrayList&lt;GraphEdge&gt;</t>
+  </si>
+  <si>
+    <t>connect(GraphVertex other, long weight)</t>
+  </si>
+  <si>
+    <t>getAdj()</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>cities: ArrayList&lt;CityIncome&gt;</t>
+  </si>
+  <si>
+    <t>toCityIncome(CityData[] c)</t>
+  </si>
+  <si>
+    <t>searchCity(String cityName)</t>
+  </si>
+  <si>
+    <t>MergeSort</t>
+  </si>
+  <si>
+    <t>aux: ArrayList&lt;Comparable&gt;</t>
+  </si>
+  <si>
+    <t>Outlook</t>
+  </si>
+  <si>
+    <t>potential: int</t>
+  </si>
+  <si>
+    <t>trend: String</t>
+  </si>
+  <si>
+    <t>getPotential()</t>
+  </si>
+  <si>
+    <t>getTrend()</t>
+  </si>
+  <si>
+    <t>OutlookData</t>
+  </si>
+  <si>
+    <t>Title: String</t>
+  </si>
+  <si>
+    <t>CPP: String</t>
+  </si>
+  <si>
+    <t>Trends: String</t>
+  </si>
+  <si>
+    <t>TrendsDate: String</t>
+  </si>
+  <si>
+    <t>Lang: String</t>
+  </si>
+  <si>
+    <t>ProvAbbr: String</t>
+  </si>
+  <si>
+    <t>Location: String</t>
+  </si>
+  <si>
+    <t>code: int</t>
+  </si>
+  <si>
+    <t>provID: int</t>
+  </si>
+  <si>
+    <t>NOC: int</t>
+  </si>
+  <si>
+    <t>cityID: int</t>
+  </si>
+  <si>
+    <t>getNOC()</t>
+  </si>
+  <si>
+    <t>getCode()</t>
+  </si>
+  <si>
+    <t>getCPP()</t>
+  </si>
+  <si>
+    <t>getLang()</t>
+  </si>
+  <si>
+    <t>getLocation()</t>
+  </si>
+  <si>
+    <t>getProvAbbr()</t>
+  </si>
+  <si>
+    <t>getProvID()</t>
+  </si>
+  <si>
+    <t>getTitle()</t>
+  </si>
+  <si>
+    <t>getTrends()</t>
+  </si>
+  <si>
+    <t>getTrendsDate()</t>
+  </si>
+  <si>
+    <t>getCityID()</t>
+  </si>
+  <si>
+    <t>Parser</t>
+  </si>
+  <si>
+    <t>outlookName: String</t>
+  </si>
+  <si>
+    <t>incomeName: String</t>
+  </si>
+  <si>
+    <t>getOutlookDataArray()</t>
+  </si>
+  <si>
+    <t>getCityDataArray()</t>
+  </si>
+  <si>
+    <t>searchIncomeCity(String jobName, String provinceCode, String aveIncome)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +495,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -303,17 +576,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,84 +968,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F36"/>
+  <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="61.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="69" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickTop="1">
+        <v>52</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
+        <v>53</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>26</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="16.5" thickTop="1" thickBot="1">
+        <v>54</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" thickTop="1" thickBot="1">
+        <v>55</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1">
+        <v>56</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" ht="15.75" thickBot="1">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1">
+        <v>57</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="15.75" thickBot="1">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -693,190 +1143,424 @@
         <v>29</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" thickTop="1">
+        <v>58</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="H9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="15.75" thickBot="1">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="F10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="15.75" thickBot="1">
+      <c r="F11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" thickTop="1">
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="15.75" thickBot="1">
+        <v>67</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="P14" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15.75" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="15.75" thickBot="1">
+      <c r="F15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15.75" thickBot="1">
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="D17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.75" thickBot="1">
+      <c r="D18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1">
-      <c r="D18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1">
+      <c r="F18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.75" thickBot="1">
       <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15.75" thickTop="1">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickTop="1">
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1">
+        <v>38</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.75" thickBot="1">
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15.75" thickTop="1">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.75" thickTop="1">
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>40</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
+        <v>41</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
+        <v>42</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.75" thickBot="1">
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1">
+      <c r="P26" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="15.75" thickBot="1">
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="D28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="D29" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="2:4">
-      <c r="D28" s="1" t="s">
+    <row r="30" spans="2:16">
+      <c r="D30" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
-      <c r="D29" s="1" t="s">
+    <row r="31" spans="2:16">
+      <c r="D31" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="2:4">
-      <c r="D30" s="1" t="s">
+    <row r="32" spans="2:16">
+      <c r="D32" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="D31" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="D32" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15.75" thickBot="1">

</xml_diff>